<commit_message>
added test case and tested untested case
</commit_message>
<xml_diff>
--- a/InTheClearTests.xlsx
+++ b/InTheClearTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshsauder/Documents/AppDevelopment/InTheClear/InTheClearTests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAFB979-5265-0D42-9F91-702CA0DBFF24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A726027A-A466-034A-BBE8-75B41D43BEBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{66150B40-FF4C-B245-A0D2-4E29E4CA51AE}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{66150B40-FF4C-B245-A0D2-4E29E4CA51AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
   <si>
     <t>Test Name</t>
   </si>
@@ -241,6 +241,21 @@
   </si>
   <si>
     <t>Both cities should be shown since they would be in different states</t>
+  </si>
+  <si>
+    <t>TB-6</t>
+  </si>
+  <si>
+    <t>Trip to a non-contiguous  IS State.</t>
+  </si>
+  <si>
+    <t>Trip should pop up an error if the route is longer than 51 hours</t>
+  </si>
+  <si>
+    <t>Trip pops up an error if longer than 51 hours</t>
+  </si>
+  <si>
+    <t>Route is given, map loads, and table still populates</t>
   </si>
 </sst>
 </file>
@@ -340,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -358,6 +373,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -674,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3046B9-C202-2842-A4E0-961B17356D10}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,18 +890,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>20</v>
+      <c r="B14" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -888,7 +909,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>20</v>
@@ -897,18 +918,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -916,35 +937,35 @@
         <v>66</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>16</v>
@@ -955,68 +976,85 @@
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
+      <c r="D24" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated excel regression tests
</commit_message>
<xml_diff>
--- a/InTheClearTests.xlsx
+++ b/InTheClearTests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshsauder/Documents/AppDevelopment/InTheClear/InTheClearTests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A726027A-A466-034A-BBE8-75B41D43BEBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CD3D4F-B27B-8445-84D3-7C048EB9526D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{66150B40-FF4C-B245-A0D2-4E29E4CA51AE}"/>
   </bookViews>
@@ -255,7 +255,7 @@
     <t>Trip pops up an error if longer than 51 hours</t>
   </si>
   <si>
-    <t>Route is given, map loads, and table still populates</t>
+    <t>Route is given, map loads, and table still populates. When Lambda function is called, a pop-up does appear.</t>
   </si>
 </sst>
 </file>
@@ -698,7 +698,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1030,7 +1030,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>49</v>
       </c>

</xml_diff>